<commit_message>
Update of the build.gradle and Organization
Update of the b
</commit_message>
<xml_diff>
--- a/Organization/PlanningPhase2.xlsx
+++ b/Organization/PlanningPhase2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaronschapira/Documents/GitHub/Project_2-1_G5/Organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A00506-6BA7-BD4C-98F0-495046458771}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE464D0-B465-8741-9546-C09BAC005C60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{61BBDE88-664B-9649-93D3-3FB53EB3984F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14800" xr2:uid="{61BBDE88-664B-9649-93D3-3FB53EB3984F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="92">
   <si>
     <t>Description</t>
   </si>
@@ -303,13 +303,19 @@
   </si>
   <si>
     <t>Adele</t>
+  </si>
+  <si>
+    <t>Genetic Algorithm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementation </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -337,6 +343,14 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -383,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -396,6 +410,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -710,20 +725,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A964446-10B4-CE41-8E76-65F705151A2F}">
-  <dimension ref="A1:J87"/>
+  <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I54" sqref="I54"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="46.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="41" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="50.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -755,12 +770,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -772,7 +787,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -781,7 +796,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -793,7 +808,7 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -802,7 +817,7 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>48</v>
       </c>
@@ -814,7 +829,7 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -826,7 +841,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -838,7 +853,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -850,7 +865,7 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -859,7 +874,7 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>50</v>
       </c>
@@ -871,7 +886,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -880,7 +895,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>47</v>
       </c>
@@ -895,7 +910,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -905,7 +920,7 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>60</v>
       </c>
@@ -920,7 +935,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -930,12 +945,12 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -945,7 +960,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -954,7 +969,7 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>43</v>
       </c>
@@ -969,12 +984,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -984,14 +999,14 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>45</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
@@ -999,22 +1014,22 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>75</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -1029,7 +1044,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -1038,7 +1053,7 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>64</v>
       </c>
@@ -1053,12 +1068,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
@@ -1068,14 +1083,14 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>45</v>
       </c>
       <c r="B29" s="3"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
@@ -1083,22 +1098,22 @@
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>77</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
         <v>46</v>
       </c>
@@ -1113,7 +1128,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="8"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1123,7 +1138,7 @@
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="8"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1133,7 +1148,7 @@
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
         <v>61</v>
       </c>
@@ -1148,7 +1163,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
         <v>44</v>
       </c>
@@ -1163,7 +1178,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
         <v>62</v>
       </c>
@@ -1178,7 +1193,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="8"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1188,7 +1203,8 @@
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="8"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -1197,9 +1213,9 @@
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="1:9">
-      <c r="A39" s="7" t="s">
-        <v>24</v>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="12" t="s">
+        <v>90</v>
       </c>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1208,166 +1224,157 @@
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
-      <c r="I39" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="7" t="s">
-        <v>55</v>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="6"/>
       <c r="H40" s="3"/>
       <c r="I40" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="A41" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="8"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
-      <c r="I41" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" s="9" t="s">
-        <v>52</v>
-      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B42" s="3"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
-      <c r="I42" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="A43" s="9" t="s">
-        <v>53</v>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" s="9" t="s">
-        <v>54</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="7" t="s">
+        <v>55</v>
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
-      <c r="G44" s="6"/>
+      <c r="G44" s="3"/>
       <c r="H44" s="3"/>
       <c r="I44" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
+        <v>51</v>
+      </c>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
-      <c r="G45" s="6"/>
+      <c r="G45" s="3"/>
       <c r="H45" s="3"/>
       <c r="I45" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46" s="9"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" s="9" t="s">
+        <v>52</v>
+      </c>
       <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
-    </row>
-    <row r="47" spans="1:9">
-      <c r="A47" s="9"/>
+      <c r="I46" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
-    </row>
-    <row r="48" spans="1:9">
-      <c r="A48" s="7" t="s">
-        <v>57</v>
+      <c r="I47" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
+      <c r="G48" s="2"/>
       <c r="H48" s="3"/>
       <c r="I48" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
-      <c r="G49" s="6"/>
+      <c r="G49" s="2"/>
       <c r="H49" s="3"/>
       <c r="I49" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10">
-      <c r="A50" s="9" t="s">
-        <v>59</v>
-      </c>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="9"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
-      <c r="F50" s="6"/>
+      <c r="F50" s="3"/>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
-      <c r="I50" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10">
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="9"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -1377,64 +1384,64 @@
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
-      <c r="G52" s="6"/>
+      <c r="G52" s="3"/>
       <c r="H52" s="3"/>
       <c r="I52" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
-      <c r="A53" s="9"/>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" s="9" t="s">
+        <v>58</v>
+      </c>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
+      <c r="G53" s="2"/>
       <c r="H53" s="3"/>
-    </row>
-    <row r="54" spans="1:10">
-      <c r="A54" s="7" t="s">
-        <v>85</v>
+      <c r="I53" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
+      <c r="F54" s="2"/>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
       <c r="I54" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10">
-      <c r="A55" s="9" t="s">
-        <v>86</v>
-      </c>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" s="9"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
-      <c r="G55" s="6"/>
+      <c r="G55" s="3"/>
       <c r="H55" s="3"/>
-      <c r="I55" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10">
-      <c r="A56" s="9" t="s">
-        <v>87</v>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="7" t="s">
+        <v>84</v>
       </c>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -1444,25 +1451,23 @@
       <c r="G56" s="6"/>
       <c r="H56" s="3"/>
       <c r="I56" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10">
-      <c r="A57" s="9" t="s">
-        <v>88</v>
-      </c>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" s="9"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
-      <c r="G57" s="6"/>
+      <c r="G57" s="3"/>
       <c r="H57" s="3"/>
-      <c r="I57" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10">
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
@@ -1470,53 +1475,56 @@
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
-    </row>
-    <row r="59" spans="1:10">
-      <c r="A59" s="2" t="s">
-        <v>41</v>
+      <c r="I58" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" s="9" t="s">
+        <v>86</v>
       </c>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
+      <c r="G59" s="6"/>
       <c r="H59" s="3"/>
-    </row>
-    <row r="60" spans="1:10">
-      <c r="A60" t="s">
-        <v>12</v>
-      </c>
-      <c r="B60" s="4"/>
-      <c r="C60" s="4"/>
-      <c r="D60" s="4"/>
-      <c r="E60" s="4"/>
-      <c r="F60" s="4"/>
-      <c r="G60" s="4"/>
-      <c r="H60" s="4"/>
-    </row>
-    <row r="61" spans="1:10">
-      <c r="A61" s="2" t="s">
-        <v>13</v>
+      <c r="I59" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="6"/>
+      <c r="H60" s="3"/>
+      <c r="I60" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" s="9" t="s">
+        <v>88</v>
       </c>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
-      <c r="G61" s="3"/>
+      <c r="G61" s="6"/>
       <c r="H61" s="3"/>
       <c r="I61" t="s">
-        <v>14</v>
-      </c>
-      <c r="J61" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10">
-      <c r="A62" s="2" t="s">
-        <v>16</v>
-      </c>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
@@ -1524,13 +1532,10 @@
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
-      <c r="I62" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10">
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -1539,28 +1544,22 @@
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
-      <c r="I63" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10">
-      <c r="A64" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
-      <c r="G64" s="3"/>
-      <c r="H64" s="3"/>
-      <c r="I64" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10">
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>12</v>
+      </c>
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
@@ -1570,12 +1569,15 @@
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
       <c r="I65" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10">
+        <v>14</v>
+      </c>
+      <c r="J65" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -1585,12 +1587,12 @@
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
       <c r="I66" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -1600,10 +1602,13 @@
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
       <c r="I67" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
@@ -1611,20 +1616,29 @@
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
-    </row>
-    <row r="69" spans="1:10">
-      <c r="A69" t="s">
-        <v>24</v>
-      </c>
-      <c r="B69" s="4"/>
-      <c r="C69" s="4"/>
-      <c r="D69" s="4"/>
-      <c r="E69" s="4"/>
-      <c r="F69" s="4"/>
-      <c r="G69" s="4"/>
-      <c r="H69" s="4"/>
-    </row>
-    <row r="70" spans="1:10">
+      <c r="I68" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
+      <c r="H69" s="3"/>
+      <c r="I69" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
@@ -1632,10 +1646,13 @@
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
-    </row>
-    <row r="71" spans="1:10">
+      <c r="I70" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -1645,125 +1662,170 @@
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
       <c r="I71" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3"/>
+      <c r="H72" s="3"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>24</v>
+      </c>
+      <c r="B73" s="4"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="4"/>
+      <c r="G73" s="4"/>
+      <c r="H73" s="4"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+      <c r="H75" s="3"/>
+      <c r="I75" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
-      <c r="A72" s="2" t="s">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I72" t="s">
+      <c r="I76" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
-      <c r="A73" s="2" t="s">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I73" t="s">
+      <c r="I77" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
-      <c r="A74" s="2" t="s">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="I74" t="s">
-        <v>30</v>
-      </c>
-      <c r="J74" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10">
-      <c r="A75" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I75" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10">
-      <c r="A77" t="s">
-        <v>33</v>
-      </c>
-      <c r="B77" t="s">
-        <v>1</v>
-      </c>
-      <c r="C77" t="s">
-        <v>2</v>
-      </c>
-      <c r="D77" t="s">
-        <v>3</v>
-      </c>
-      <c r="E77" t="s">
-        <v>4</v>
-      </c>
-      <c r="F77" t="s">
-        <v>5</v>
-      </c>
-      <c r="G77" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10">
-      <c r="A78" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="I78" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="79" spans="1:10">
+      <c r="J78" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I79" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
-      <c r="A80" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I80" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9">
-      <c r="A81" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I81" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>33</v>
+      </c>
+      <c r="B81" t="s">
+        <v>1</v>
+      </c>
+      <c r="C81" t="s">
+        <v>2</v>
+      </c>
+      <c r="D81" t="s">
+        <v>3</v>
+      </c>
+      <c r="E81" t="s">
+        <v>4</v>
+      </c>
+      <c r="F81" t="s">
+        <v>5</v>
+      </c>
+      <c r="G81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="I82" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="I83" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I84" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A85" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I85" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A86" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I86" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A87" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I87" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A88" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I84" t="s">
+      <c r="I88" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="87" spans="1:9">
-      <c r="A87" s="6" t="s">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A91" s="6" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>